<commit_message>
June 16 Data Update
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9542BE3-013B-4E12-A7A6-4F33FEFBC088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D4BFE-B15A-44F0-BC64-F496B912CE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12774,11 +12774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13244,7 +13244,7 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -14085,7 +14085,7 @@
         <v>2</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -14578,7 +14578,7 @@
         <v>2</v>
       </c>
       <c r="I62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -14662,10 +14662,10 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="I65">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -14691,10 +14691,10 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="I66">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -14720,10 +14720,10 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="I67">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -15126,10 +15126,10 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I81">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -15155,10 +15155,10 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I82">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -15271,10 +15271,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I86">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -16115,7 +16115,7 @@
         <v>7</v>
       </c>
       <c r="I115">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -17072,7 +17072,7 @@
         <v>8</v>
       </c>
       <c r="I148">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
@@ -17507,7 +17507,7 @@
         <v>6</v>
       </c>
       <c r="I163">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.35">
@@ -17971,7 +17971,7 @@
         <v>8</v>
       </c>
       <c r="I179">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.35">
@@ -18000,7 +18000,7 @@
         <v>2</v>
       </c>
       <c r="I180">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.35">
@@ -18841,7 +18841,7 @@
         <v>4</v>
       </c>
       <c r="I209">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.35">
@@ -19363,7 +19363,7 @@
         <v>2</v>
       </c>
       <c r="I227">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.35">
@@ -22608,10 +22608,10 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I339">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.35">
@@ -24844,7 +24844,7 @@
         <v>4</v>
       </c>
       <c r="I416">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.35">
@@ -25656,7 +25656,7 @@
         <v>3</v>
       </c>
       <c r="I444">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:9" x14ac:dyDescent="0.35">
@@ -25914,10 +25914,10 @@
         <v>1</v>
       </c>
       <c r="H453">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I453">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.35">
@@ -27886,10 +27886,10 @@
         <v>1</v>
       </c>
       <c r="H521">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="I521">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="522" spans="1:9" x14ac:dyDescent="0.35">
@@ -27918,7 +27918,7 @@
         <v>14</v>
       </c>
       <c r="I522">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="523" spans="1:9" x14ac:dyDescent="0.35">
@@ -28901,10 +28901,10 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I556">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.35">
@@ -29220,10 +29220,10 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="I567">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.35">
@@ -29510,10 +29510,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="I577">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29539,10 +29539,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="I578">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29568,10 +29568,10 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="I579">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -29655,10 +29655,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="I582">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29887,10 +29887,10 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="I590">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -29916,10 +29916,10 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="I591">
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -30061,10 +30061,10 @@
         <v>1</v>
       </c>
       <c r="H596">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I596">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="597" spans="1:9" x14ac:dyDescent="0.35">
@@ -31308,10 +31308,10 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I639">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -31337,10 +31337,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I640">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31366,10 +31366,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>192</v>
+        <v>133</v>
       </c>
       <c r="I641">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32410,10 +32410,10 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="I677">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -32529,7 +32529,7 @@
         <v>84</v>
       </c>
       <c r="I681">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -33193,10 +33193,10 @@
         <v>1</v>
       </c>
       <c r="H704">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I704">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="705" spans="1:9" x14ac:dyDescent="0.35">
@@ -33428,7 +33428,7 @@
         <v>3</v>
       </c>
       <c r="I712">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.35">
@@ -33976,10 +33976,10 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I731">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -34005,10 +34005,10 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I732">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -34034,10 +34034,10 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I733">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -34063,10 +34063,10 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I734">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -34089,13 +34089,13 @@
         <v>3</v>
       </c>
       <c r="G735">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H735">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I735">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.35">
@@ -34121,10 +34121,10 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I736">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.35">
@@ -34150,7 +34150,7 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I737">
         <v>3</v>
@@ -34208,10 +34208,10 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="I739">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.35">
@@ -34556,10 +34556,10 @@
         <v>1</v>
       </c>
       <c r="H751">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I751">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="752" spans="1:9" x14ac:dyDescent="0.35">
@@ -34588,7 +34588,7 @@
         <v>6</v>
       </c>
       <c r="I752">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.35">
@@ -34614,10 +34614,10 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I753">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -34643,10 +34643,10 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I754">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="755" spans="1:9" x14ac:dyDescent="0.35">
@@ -34875,7 +34875,7 @@
         <v>1</v>
       </c>
       <c r="H762">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I762">
         <v>4</v>
@@ -35197,7 +35197,7 @@
         <v>18</v>
       </c>
       <c r="I773">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="774" spans="1:9" x14ac:dyDescent="0.35">
@@ -35255,7 +35255,7 @@
         <v>3</v>
       </c>
       <c r="I775">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="776" spans="1:9" x14ac:dyDescent="0.35">
@@ -35313,7 +35313,7 @@
         <v>7</v>
       </c>
       <c r="I777">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.35">
@@ -35948,10 +35948,10 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="I799">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.35">
@@ -35977,10 +35977,10 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I800">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="801" spans="1:9" x14ac:dyDescent="0.35">
@@ -36064,10 +36064,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I803">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -36093,10 +36093,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I804">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -37572,10 +37572,10 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I855">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.35">
@@ -37746,10 +37746,10 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I861">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -38297,10 +38297,10 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="I880">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -39022,10 +39022,10 @@
         <v>1</v>
       </c>
       <c r="H905">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I905">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.35">
@@ -39138,10 +39138,10 @@
         <v>1</v>
       </c>
       <c r="H909">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I909">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.35">
@@ -39167,10 +39167,10 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="I910">
-        <v>95</v>
+        <v>18</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.35">
@@ -39196,10 +39196,10 @@
         <v>1</v>
       </c>
       <c r="H911">
-        <v>283</v>
+        <v>137</v>
       </c>
       <c r="I911">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.35">
@@ -39402,7 +39402,7 @@
         <v>19</v>
       </c>
       <c r="I918">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.35">
@@ -39660,10 +39660,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="I927">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -39776,10 +39776,10 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I931">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="932" spans="1:9" x14ac:dyDescent="0.35">
@@ -40124,10 +40124,10 @@
         <v>1</v>
       </c>
       <c r="H943">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I943">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="944" spans="1:9" x14ac:dyDescent="0.35">
@@ -40762,10 +40762,10 @@
         <v>1</v>
       </c>
       <c r="H965">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I965">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="966" spans="1:9" x14ac:dyDescent="0.35">
@@ -41168,10 +41168,10 @@
         <v>1</v>
       </c>
       <c r="H979">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I979">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="980" spans="1:9" x14ac:dyDescent="0.35">
@@ -41197,10 +41197,10 @@
         <v>1</v>
       </c>
       <c r="H980">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I980">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="981" spans="1:9" x14ac:dyDescent="0.35">
@@ -41229,7 +41229,7 @@
         <v>4</v>
       </c>
       <c r="I981">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.35">
@@ -41458,10 +41458,10 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="I989">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.35">
@@ -41661,10 +41661,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="I996">
-        <v>75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -41719,10 +41719,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I998">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -44535,7 +44535,7 @@
         <v>3</v>
       </c>
       <c r="I1095">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1096" spans="1:9" x14ac:dyDescent="0.35">
@@ -44619,10 +44619,10 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="I1098">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1099" spans="1:9" x14ac:dyDescent="0.35">
@@ -44735,10 +44735,10 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="I1102">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.35">
@@ -45025,10 +45025,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>126</v>
+        <v>58</v>
       </c>
       <c r="I1112">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">
@@ -45373,7 +45373,7 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I1124">
         <v>5</v>
@@ -45402,7 +45402,7 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I1125">
         <v>1</v>
@@ -45431,10 +45431,10 @@
         <v>1</v>
       </c>
       <c r="H1126">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1126">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1127" spans="1:9" x14ac:dyDescent="0.35">
@@ -45460,10 +45460,10 @@
         <v>0</v>
       </c>
       <c r="H1127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I1127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1128" spans="1:9" x14ac:dyDescent="0.35">
@@ -45489,10 +45489,10 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I1128">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1129" spans="1:9" x14ac:dyDescent="0.35">
@@ -45692,10 +45692,10 @@
         <v>1</v>
       </c>
       <c r="H1135">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="I1135">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1136" spans="1:9" x14ac:dyDescent="0.35">
@@ -46011,10 +46011,10 @@
         <v>1</v>
       </c>
       <c r="H1146">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I1146">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1147" spans="1:9" x14ac:dyDescent="0.35">
@@ -46069,10 +46069,10 @@
         <v>1</v>
       </c>
       <c r="H1148">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I1148">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1149" spans="1:9" x14ac:dyDescent="0.35">
@@ -46501,13 +46501,13 @@
         <v>3</v>
       </c>
       <c r="G1163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1163">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I1163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1164" spans="1:9" x14ac:dyDescent="0.35">
@@ -47896,10 +47896,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="I1211">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
June 16 Data Update (#5)
First time Alyson makes it through the automated process
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9542BE3-013B-4E12-A7A6-4F33FEFBC088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D4BFE-B15A-44F0-BC64-F496B912CE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12774,11 +12774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13244,7 +13244,7 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -14085,7 +14085,7 @@
         <v>2</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -14578,7 +14578,7 @@
         <v>2</v>
       </c>
       <c r="I62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -14662,10 +14662,10 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="I65">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -14691,10 +14691,10 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="I66">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -14720,10 +14720,10 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="I67">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -15126,10 +15126,10 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I81">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -15155,10 +15155,10 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I82">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -15271,10 +15271,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I86">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -16115,7 +16115,7 @@
         <v>7</v>
       </c>
       <c r="I115">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -17072,7 +17072,7 @@
         <v>8</v>
       </c>
       <c r="I148">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
@@ -17507,7 +17507,7 @@
         <v>6</v>
       </c>
       <c r="I163">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.35">
@@ -17971,7 +17971,7 @@
         <v>8</v>
       </c>
       <c r="I179">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.35">
@@ -18000,7 +18000,7 @@
         <v>2</v>
       </c>
       <c r="I180">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.35">
@@ -18841,7 +18841,7 @@
         <v>4</v>
       </c>
       <c r="I209">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.35">
@@ -19363,7 +19363,7 @@
         <v>2</v>
       </c>
       <c r="I227">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.35">
@@ -22608,10 +22608,10 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I339">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.35">
@@ -24844,7 +24844,7 @@
         <v>4</v>
       </c>
       <c r="I416">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.35">
@@ -25656,7 +25656,7 @@
         <v>3</v>
       </c>
       <c r="I444">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:9" x14ac:dyDescent="0.35">
@@ -25914,10 +25914,10 @@
         <v>1</v>
       </c>
       <c r="H453">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I453">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.35">
@@ -27886,10 +27886,10 @@
         <v>1</v>
       </c>
       <c r="H521">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="I521">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="522" spans="1:9" x14ac:dyDescent="0.35">
@@ -27918,7 +27918,7 @@
         <v>14</v>
       </c>
       <c r="I522">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="523" spans="1:9" x14ac:dyDescent="0.35">
@@ -28901,10 +28901,10 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I556">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.35">
@@ -29220,10 +29220,10 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="I567">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.35">
@@ -29510,10 +29510,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="I577">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29539,10 +29539,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="I578">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29568,10 +29568,10 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="I579">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -29655,10 +29655,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="I582">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29887,10 +29887,10 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="I590">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -29916,10 +29916,10 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="I591">
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -30061,10 +30061,10 @@
         <v>1</v>
       </c>
       <c r="H596">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I596">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="597" spans="1:9" x14ac:dyDescent="0.35">
@@ -31308,10 +31308,10 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I639">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -31337,10 +31337,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I640">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31366,10 +31366,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>192</v>
+        <v>133</v>
       </c>
       <c r="I641">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32410,10 +32410,10 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="I677">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -32529,7 +32529,7 @@
         <v>84</v>
       </c>
       <c r="I681">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -33193,10 +33193,10 @@
         <v>1</v>
       </c>
       <c r="H704">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I704">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="705" spans="1:9" x14ac:dyDescent="0.35">
@@ -33428,7 +33428,7 @@
         <v>3</v>
       </c>
       <c r="I712">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.35">
@@ -33976,10 +33976,10 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I731">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -34005,10 +34005,10 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I732">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -34034,10 +34034,10 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I733">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -34063,10 +34063,10 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I734">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -34089,13 +34089,13 @@
         <v>3</v>
       </c>
       <c r="G735">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H735">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I735">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.35">
@@ -34121,10 +34121,10 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I736">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.35">
@@ -34150,7 +34150,7 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I737">
         <v>3</v>
@@ -34208,10 +34208,10 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="I739">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.35">
@@ -34556,10 +34556,10 @@
         <v>1</v>
       </c>
       <c r="H751">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I751">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="752" spans="1:9" x14ac:dyDescent="0.35">
@@ -34588,7 +34588,7 @@
         <v>6</v>
       </c>
       <c r="I752">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.35">
@@ -34614,10 +34614,10 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I753">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -34643,10 +34643,10 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I754">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="755" spans="1:9" x14ac:dyDescent="0.35">
@@ -34875,7 +34875,7 @@
         <v>1</v>
       </c>
       <c r="H762">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I762">
         <v>4</v>
@@ -35197,7 +35197,7 @@
         <v>18</v>
       </c>
       <c r="I773">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="774" spans="1:9" x14ac:dyDescent="0.35">
@@ -35255,7 +35255,7 @@
         <v>3</v>
       </c>
       <c r="I775">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="776" spans="1:9" x14ac:dyDescent="0.35">
@@ -35313,7 +35313,7 @@
         <v>7</v>
       </c>
       <c r="I777">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.35">
@@ -35948,10 +35948,10 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="I799">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.35">
@@ -35977,10 +35977,10 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I800">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="801" spans="1:9" x14ac:dyDescent="0.35">
@@ -36064,10 +36064,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I803">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -36093,10 +36093,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I804">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -37572,10 +37572,10 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I855">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.35">
@@ -37746,10 +37746,10 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I861">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -38297,10 +38297,10 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="I880">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -39022,10 +39022,10 @@
         <v>1</v>
       </c>
       <c r="H905">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I905">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.35">
@@ -39138,10 +39138,10 @@
         <v>1</v>
       </c>
       <c r="H909">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I909">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.35">
@@ -39167,10 +39167,10 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="I910">
-        <v>95</v>
+        <v>18</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.35">
@@ -39196,10 +39196,10 @@
         <v>1</v>
       </c>
       <c r="H911">
-        <v>283</v>
+        <v>137</v>
       </c>
       <c r="I911">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.35">
@@ -39402,7 +39402,7 @@
         <v>19</v>
       </c>
       <c r="I918">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.35">
@@ -39660,10 +39660,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="I927">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -39776,10 +39776,10 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I931">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="932" spans="1:9" x14ac:dyDescent="0.35">
@@ -40124,10 +40124,10 @@
         <v>1</v>
       </c>
       <c r="H943">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I943">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="944" spans="1:9" x14ac:dyDescent="0.35">
@@ -40762,10 +40762,10 @@
         <v>1</v>
       </c>
       <c r="H965">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I965">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="966" spans="1:9" x14ac:dyDescent="0.35">
@@ -41168,10 +41168,10 @@
         <v>1</v>
       </c>
       <c r="H979">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I979">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="980" spans="1:9" x14ac:dyDescent="0.35">
@@ -41197,10 +41197,10 @@
         <v>1</v>
       </c>
       <c r="H980">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I980">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="981" spans="1:9" x14ac:dyDescent="0.35">
@@ -41229,7 +41229,7 @@
         <v>4</v>
       </c>
       <c r="I981">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.35">
@@ -41458,10 +41458,10 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="I989">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.35">
@@ -41661,10 +41661,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="I996">
-        <v>75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -41719,10 +41719,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I998">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -44535,7 +44535,7 @@
         <v>3</v>
       </c>
       <c r="I1095">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1096" spans="1:9" x14ac:dyDescent="0.35">
@@ -44619,10 +44619,10 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="I1098">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1099" spans="1:9" x14ac:dyDescent="0.35">
@@ -44735,10 +44735,10 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="I1102">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.35">
@@ -45025,10 +45025,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>126</v>
+        <v>58</v>
       </c>
       <c r="I1112">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">
@@ -45373,7 +45373,7 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I1124">
         <v>5</v>
@@ -45402,7 +45402,7 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I1125">
         <v>1</v>
@@ -45431,10 +45431,10 @@
         <v>1</v>
       </c>
       <c r="H1126">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1126">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1127" spans="1:9" x14ac:dyDescent="0.35">
@@ -45460,10 +45460,10 @@
         <v>0</v>
       </c>
       <c r="H1127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I1127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1128" spans="1:9" x14ac:dyDescent="0.35">
@@ -45489,10 +45489,10 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I1128">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1129" spans="1:9" x14ac:dyDescent="0.35">
@@ -45692,10 +45692,10 @@
         <v>1</v>
       </c>
       <c r="H1135">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="I1135">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1136" spans="1:9" x14ac:dyDescent="0.35">
@@ -46011,10 +46011,10 @@
         <v>1</v>
       </c>
       <c r="H1146">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I1146">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1147" spans="1:9" x14ac:dyDescent="0.35">
@@ -46069,10 +46069,10 @@
         <v>1</v>
       </c>
       <c r="H1148">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I1148">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1149" spans="1:9" x14ac:dyDescent="0.35">
@@ -46501,13 +46501,13 @@
         <v>3</v>
       </c>
       <c r="G1163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1163">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I1163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1164" spans="1:9" x14ac:dyDescent="0.35">
@@ -47896,10 +47896,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="I1211">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Use new columns AMO and UPI
The Daily Total and Shift Total columns are now replaced by
Approved Max Occupancy and Unique PIs.
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D4BFE-B15A-44F0-BC64-F496B912CE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6176234-38F4-4D1F-BD8D-BC15A7C69DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11929,10 +11929,10 @@
     <t>Research Building</t>
   </si>
   <si>
-    <t>Daily Total</t>
-  </si>
-  <si>
-    <t>Shift Total</t>
+    <t>AMO</t>
+  </si>
+  <si>
+    <t>UPI</t>
   </si>
 </sst>
 </file>
@@ -12778,7 +12778,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Use new columns AMO and UPI (#7)
The Daily Total and Shift Total columns/variables are now replaced by
Approved Max Occupancy and Unique PIs.

Closes #6.
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D4BFE-B15A-44F0-BC64-F496B912CE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6176234-38F4-4D1F-BD8D-BC15A7C69DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11929,10 +11929,10 @@
     <t>Research Building</t>
   </si>
   <si>
-    <t>Daily Total</t>
-  </si>
-  <si>
-    <t>Shift Total</t>
+    <t>AMO</t>
+  </si>
+  <si>
+    <t>UPI</t>
   </si>
 </sst>
 </file>
@@ -12778,7 +12778,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
June 18 data update
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D4BFE-B15A-44F0-BC64-F496B912CE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E659C71-FB5A-4425-B97F-FBB8A8C4EE6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11929,16 +11929,16 @@
     <t>Research Building</t>
   </si>
   <si>
-    <t>Daily Total</t>
-  </si>
-  <si>
-    <t>Shift Total</t>
+    <t>AMO</t>
+  </si>
+  <si>
+    <t>UPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12416,10 +12416,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -12774,11 +12773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12805,7 +12804,7 @@
       <c r="G1" s="1" t="s">
         <v>3968</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>3969</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -13325,13 +13324,13 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -15155,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -29510,7 +29509,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I577">
         <v>24</v>
@@ -37572,7 +37571,7 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I855">
         <v>4</v>
@@ -41110,10 +41109,10 @@
         <v>1</v>
       </c>
       <c r="H977">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I977">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="978" spans="1:9" x14ac:dyDescent="0.35">
@@ -41139,10 +41138,10 @@
         <v>1</v>
       </c>
       <c r="H978">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I978">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="979" spans="1:9" x14ac:dyDescent="0.35">
@@ -45489,10 +45488,10 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I1128">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1129" spans="1:9" x14ac:dyDescent="0.35">
@@ -48310,5 +48309,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
July 18 new data, attempt 3 (#10)
* Add files via upload

* Add files via upload
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6176234-38F4-4D1F-BD8D-BC15A7C69DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA714EC5-6F1A-45E8-A196-99C83B89CF0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -12416,10 +12416,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -12778,7 +12777,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12805,7 +12804,7 @@
       <c r="G1" s="1" t="s">
         <v>3968</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>3969</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -13325,13 +13324,13 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -15155,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -29510,7 +29509,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I577">
         <v>24</v>
@@ -37572,7 +37571,7 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I855">
         <v>4</v>
@@ -41110,10 +41109,10 @@
         <v>1</v>
       </c>
       <c r="H977">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I977">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="978" spans="1:9" x14ac:dyDescent="0.35">
@@ -41139,10 +41138,10 @@
         <v>1</v>
       </c>
       <c r="H978">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I978">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="979" spans="1:9" x14ac:dyDescent="0.35">
@@ -45489,10 +45488,10 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I1128">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1129" spans="1:9" x14ac:dyDescent="0.35">
@@ -48310,5 +48309,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add files via upload (#12)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\GitHub\campus-research-reopening\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA714EC5-6F1A-45E8-A196-99C83B89CF0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A1F0D4B-24CD-4348-AE65-6EBC51736E0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12773,7 +12773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -14693,7 +14693,7 @@
         <v>12</v>
       </c>
       <c r="I66">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -14722,7 +14722,7 @@
         <v>22</v>
       </c>
       <c r="I67">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -28903,7 +28903,7 @@
         <v>14</v>
       </c>
       <c r="I556">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.35">
@@ -29222,7 +29222,7 @@
         <v>23</v>
       </c>
       <c r="I567">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.35">
@@ -29538,10 +29538,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I578">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29654,10 +29654,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="I582">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29886,10 +29886,10 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I590">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -31307,10 +31307,10 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I639">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -32525,7 +32525,7 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="I681">
         <v>20</v>
@@ -34207,10 +34207,10 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I739">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.35">
@@ -35947,7 +35947,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I799">
         <v>19</v>
@@ -38299,7 +38299,7 @@
         <v>104</v>
       </c>
       <c r="I880">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -41457,10 +41457,10 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I989">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.35">
@@ -41660,10 +41660,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I996">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -45024,10 +45024,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I1112">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">
@@ -47895,10 +47895,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I1211">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">
@@ -48309,6 +48309,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add files via upload (#13)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A1F0D4B-24CD-4348-AE65-6EBC51736E0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70FCC94E-1551-4818-BCBC-C20188EA6C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -5974,10 +5974,10 @@
     <t>110 Dan Allen Dr.</t>
   </si>
   <si>
-    <t>Daniels Hall</t>
-  </si>
-  <si>
-    <t>DAN</t>
+    <t>111 Lampe Drive</t>
+  </si>
+  <si>
+    <t>LMP</t>
   </si>
   <si>
     <t>111 Lampe Dr.</t>
@@ -14719,10 +14719,10 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I67">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -15154,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -29512,7 +29512,7 @@
         <v>51</v>
       </c>
       <c r="I577">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29541,7 +29541,7 @@
         <v>125</v>
       </c>
       <c r="I578">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -30060,7 +30060,7 @@
         <v>1</v>
       </c>
       <c r="H596">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I596">
         <v>2</v>
@@ -32525,10 +32525,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I681">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -44734,7 +44734,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I1102">
         <v>29</v>

</xml_diff>

<commit_message>
Add files via upload (#14)
New data on June 29
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70FCC94E-1551-4818-BCBC-C20188EA6C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C23E1921-F972-484F-8DEA-94FA70406FEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12773,14 +12773,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
+      <selection activeCell="A681" sqref="A681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="65.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -14693,7 +14696,7 @@
         <v>12</v>
       </c>
       <c r="I66">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -29509,7 +29512,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I577">
         <v>25</v>
@@ -29538,10 +29541,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I578">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29886,7 +29889,7 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I590">
         <v>7</v>
@@ -31307,10 +31310,10 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I639">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -31336,10 +31339,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I640">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31365,7 +31368,7 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I641">
         <v>45</v>
@@ -32525,7 +32528,7 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I681">
         <v>21</v>
@@ -34584,10 +34587,10 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I752">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.35">
@@ -36063,10 +36066,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I803">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -38296,10 +38299,10 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I880">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -39398,10 +39401,10 @@
         <v>1</v>
       </c>
       <c r="H918">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="I918">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.35">
@@ -41080,10 +41083,10 @@
         <v>1</v>
       </c>
       <c r="H976">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I976">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="977" spans="1:9" x14ac:dyDescent="0.35">
@@ -41167,10 +41170,10 @@
         <v>1</v>
       </c>
       <c r="H979">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I979">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="980" spans="1:9" x14ac:dyDescent="0.35">
@@ -41718,10 +41721,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I998">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -43165,13 +43168,13 @@
         <v>3</v>
       </c>
       <c r="G1048">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1048">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1048">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1049" spans="1:9" x14ac:dyDescent="0.35">
@@ -45024,10 +45027,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I1112">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#15)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C23E1921-F972-484F-8DEA-94FA70406FEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCA9909-C048-461E-AB24-2EDCEE043C51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12773,17 +12773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
-      <selection activeCell="A681" sqref="A681"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="65.81640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -13330,10 +13327,10 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -14664,7 +14661,7 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>14</v>
@@ -14693,7 +14690,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I66">
         <v>13</v>
@@ -14722,7 +14719,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -15128,7 +15125,7 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I81">
         <v>6</v>
@@ -15157,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -15273,10 +15270,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I86">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -29512,10 +29509,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="I577">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29541,7 +29538,7 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="I578">
         <v>25</v>
@@ -29570,7 +29567,7 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="I579">
         <v>10</v>
@@ -29657,10 +29654,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="I582">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29918,10 +29915,10 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I591">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -31310,7 +31307,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="I639">
         <v>26</v>
@@ -31339,7 +31336,7 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I640">
         <v>10</v>
@@ -31368,7 +31365,7 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="I641">
         <v>45</v>
@@ -32412,10 +32409,10 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I677">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -32528,10 +32525,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="I681">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -33134,13 +33131,13 @@
         <v>3</v>
       </c>
       <c r="G702">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H702">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I702">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.35">
@@ -33337,13 +33334,13 @@
         <v>3</v>
       </c>
       <c r="G709">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H709">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I709">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="710" spans="1:9" x14ac:dyDescent="0.35">
@@ -33978,10 +33975,10 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I731">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -34007,10 +34004,10 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I732">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -34036,10 +34033,10 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I733">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -34065,10 +34062,10 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I734">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -34210,7 +34207,7 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="I739">
         <v>6</v>
@@ -34587,7 +34584,7 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I752">
         <v>5</v>
@@ -34616,10 +34613,10 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I753">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -34645,7 +34642,7 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I754">
         <v>4</v>
@@ -35950,7 +35947,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="I799">
         <v>19</v>
@@ -35979,7 +35976,7 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I800">
         <v>4</v>
@@ -36066,7 +36063,7 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I803">
         <v>2</v>
@@ -36095,10 +36092,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I804">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -39633,10 +39630,10 @@
         <v>1</v>
       </c>
       <c r="H926">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I926">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="927" spans="1:9" x14ac:dyDescent="0.35">
@@ -39662,10 +39659,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I927">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -41721,10 +41718,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I998">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -45375,10 +45372,10 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I1124">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1125" spans="1:9" x14ac:dyDescent="0.35">
@@ -47898,10 +47895,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I1211">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#16)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCA9909-C048-461E-AB24-2EDCEE043C51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA08CAB4-A96B-4701-9A20-406C1E1AE682}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12777,10 +12777,13 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="65.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -13327,10 +13330,10 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -14661,7 +14664,7 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I65">
         <v>14</v>
@@ -14690,7 +14693,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I66">
         <v>13</v>
@@ -14719,7 +14722,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -15125,7 +15128,7 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I81">
         <v>6</v>
@@ -15154,7 +15157,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -15270,10 +15273,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I86">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -29509,10 +29512,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="I577">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29538,7 +29541,7 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="I578">
         <v>25</v>
@@ -29567,7 +29570,7 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="I579">
         <v>10</v>
@@ -29654,10 +29657,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="I582">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29915,10 +29918,10 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I591">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -31307,7 +31310,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="I639">
         <v>26</v>
@@ -31336,7 +31339,7 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I640">
         <v>10</v>
@@ -31365,7 +31368,7 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="I641">
         <v>45</v>
@@ -32409,10 +32412,10 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I677">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -32525,10 +32528,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I681">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -33131,13 +33134,13 @@
         <v>3</v>
       </c>
       <c r="G702">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H702">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I702">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.35">
@@ -33334,13 +33337,13 @@
         <v>3</v>
       </c>
       <c r="G709">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H709">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I709">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:9" x14ac:dyDescent="0.35">
@@ -33975,10 +33978,10 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I731">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -34004,10 +34007,10 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I732">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -34033,10 +34036,10 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I733">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -34062,10 +34065,10 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I734">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -34207,7 +34210,7 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I739">
         <v>6</v>
@@ -34584,7 +34587,7 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I752">
         <v>5</v>
@@ -34613,10 +34616,10 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I753">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -34642,7 +34645,7 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I754">
         <v>4</v>
@@ -35947,7 +35950,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I799">
         <v>19</v>
@@ -35976,7 +35979,7 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I800">
         <v>4</v>
@@ -36063,7 +36066,7 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I803">
         <v>2</v>
@@ -36092,10 +36095,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I804">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -39630,10 +39633,10 @@
         <v>1</v>
       </c>
       <c r="H926">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I926">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="927" spans="1:9" x14ac:dyDescent="0.35">
@@ -39659,10 +39662,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I927">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -41718,10 +41721,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I998">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -45372,10 +45375,10 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I1124">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1125" spans="1:9" x14ac:dyDescent="0.35">
@@ -47895,10 +47898,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I1211">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#17)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA08CAB4-A96B-4701-9A20-406C1E1AE682}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0252447F-FD69-4656-BB84-66E55CE12CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12777,13 +12777,10 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="65.81640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -13333,7 +13330,7 @@
         <v>6</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -14664,10 +14661,10 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I65">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -14693,7 +14690,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I66">
         <v>13</v>
@@ -15273,10 +15270,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I86">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -25916,10 +25913,10 @@
         <v>1</v>
       </c>
       <c r="H453">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I453">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.35">
@@ -29515,7 +29512,7 @@
         <v>52</v>
       </c>
       <c r="I577">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29541,7 +29538,7 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I578">
         <v>25</v>
@@ -29660,7 +29657,7 @@
         <v>117</v>
       </c>
       <c r="I582">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29918,10 +29915,10 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I591">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -31371,7 +31368,7 @@
         <v>134</v>
       </c>
       <c r="I641">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32412,10 +32409,10 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="I677">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -32528,10 +32525,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I681">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -33134,13 +33131,13 @@
         <v>3</v>
       </c>
       <c r="G702">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H702">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I702">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.35">
@@ -33337,13 +33334,13 @@
         <v>3</v>
       </c>
       <c r="G709">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H709">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I709">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="710" spans="1:9" x14ac:dyDescent="0.35">
@@ -33978,10 +33975,10 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I731">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -34007,10 +34004,10 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I732">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -34036,10 +34033,10 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I733">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -34065,10 +34062,10 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I734">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -34616,10 +34613,10 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I753">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -35950,7 +35947,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I799">
         <v>19</v>
@@ -36095,10 +36092,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I804">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -39633,10 +39630,10 @@
         <v>1</v>
       </c>
       <c r="H926">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I926">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="927" spans="1:9" x14ac:dyDescent="0.35">
@@ -39662,10 +39659,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I927">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -41721,10 +41718,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I998">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -44737,7 +44734,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I1102">
         <v>29</v>
@@ -45027,7 +45024,7 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I1112">
         <v>16</v>
@@ -45375,10 +45372,10 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I1124">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1125" spans="1:9" x14ac:dyDescent="0.35">
@@ -47898,10 +47895,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I1211">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">
@@ -48312,5 +48309,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add files via upload (#18)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0252447F-FD69-4656-BB84-66E55CE12CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DE7BAA2-613D-40EB-888B-61ACD64FF765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12777,12 +12777,12 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3962</v>
       </c>
@@ -28903,7 +28903,7 @@
         <v>14</v>
       </c>
       <c r="I556">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.35">
@@ -29509,7 +29509,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I577">
         <v>23</v>
@@ -29538,10 +29538,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I578">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29886,10 +29886,10 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I590">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -31368,7 +31368,7 @@
         <v>134</v>
       </c>
       <c r="I641">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -36066,7 +36066,7 @@
         <v>24</v>
       </c>
       <c r="I803">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -41457,10 +41457,10 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I989">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#19)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DE7BAA2-613D-40EB-888B-61ACD64FF765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65F668F0-ACED-4D6C-BDE3-800262E2F018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12777,7 +12777,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41718,10 +41718,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I998">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -47895,7 +47895,7 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1211">
         <v>31</v>

</xml_diff>

<commit_message>
Add files via upload (#20)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65F668F0-ACED-4D6C-BDE3-800262E2F018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C53EB4B1-FBA3-4F21-B0A0-82820A15977C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12776,13 +12776,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A995" workbookViewId="0">
+      <selection activeCell="A998" sqref="A998:XFD998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3962</v>
       </c>
@@ -15154,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="I82">
         <v>5</v>
@@ -28900,7 +28900,7 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I556">
         <v>9</v>
@@ -29538,7 +29538,7 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I578">
         <v>26</v>
@@ -29567,10 +29567,10 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I579">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -29886,7 +29886,7 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I590">
         <v>8</v>
@@ -31307,7 +31307,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I639">
         <v>26</v>
@@ -31336,10 +31336,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I640">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31365,10 +31365,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="I641">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32525,10 +32525,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="I681">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -34091,10 +34091,10 @@
         <v>1</v>
       </c>
       <c r="H735">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I735">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.35">
@@ -34120,10 +34120,10 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I736">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.35">
@@ -34149,10 +34149,10 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I737">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="738" spans="1:9" x14ac:dyDescent="0.35">
@@ -36063,10 +36063,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I803">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -39166,7 +39166,7 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I910">
         <v>18</v>
@@ -41660,10 +41660,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I996">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -41718,10 +41718,10 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="I998">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.35">
@@ -44734,7 +44734,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I1102">
         <v>29</v>
@@ -45691,7 +45691,7 @@
         <v>1</v>
       </c>
       <c r="H1135">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I1135">
         <v>9</v>
@@ -47895,10 +47895,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I1211">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#21)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C53EB4B1-FBA3-4F21-B0A0-82820A15977C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3624DC2-7145-4B73-AC25-810CA18DD3C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12416,9 +12416,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -12776,38 +12775,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A995" workbookViewId="0">
-      <selection activeCell="A998" sqref="A998:XFD998"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>3962</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>3963</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>3964</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3965</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3966</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3967</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>3968</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>3969</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>3970</v>
       </c>
     </row>
@@ -14661,10 +14660,10 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I65">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -14719,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -15270,10 +15269,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I86">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -28900,7 +28899,7 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I556">
         <v>9</v>
@@ -29509,10 +29508,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I577">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29567,10 +29566,10 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="I579">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -29973,10 +29972,10 @@
         <v>1</v>
       </c>
       <c r="H593">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I593">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="594" spans="1:9" x14ac:dyDescent="0.35">
@@ -31307,10 +31306,10 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="I639">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -36092,10 +36091,10 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I804">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -37049,10 +37048,10 @@
         <v>1</v>
       </c>
       <c r="H837">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I837">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="838" spans="1:9" x14ac:dyDescent="0.35">
@@ -39137,7 +39136,7 @@
         <v>1</v>
       </c>
       <c r="H909">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I909">
         <v>2</v>
@@ -41167,7 +41166,7 @@
         <v>1</v>
       </c>
       <c r="H979">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I979">
         <v>5</v>
@@ -41660,10 +41659,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I996">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -44383,13 +44382,13 @@
         <v>3</v>
       </c>
       <c r="G1090">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1090">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I1090">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1091" spans="1:9" x14ac:dyDescent="0.35">
@@ -45894,10 +45893,10 @@
         <v>1</v>
       </c>
       <c r="H1142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1143" spans="1:9" x14ac:dyDescent="0.35">
@@ -45981,10 +45980,10 @@
         <v>1</v>
       </c>
       <c r="H1145">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I1145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1146" spans="1:9" x14ac:dyDescent="0.35">
@@ -46384,13 +46383,13 @@
         <v>3</v>
       </c>
       <c r="G1159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I1159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1160" spans="1:9" x14ac:dyDescent="0.35">
@@ -47895,7 +47894,7 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1211">
         <v>32</v>
@@ -48309,6 +48308,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add files via upload (#23)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3624DC2-7145-4B73-AC25-810CA18DD3C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45869B6E-444E-4127-B407-691C47D178B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12772,11 +12772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13329,7 +13329,7 @@
         <v>6</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -14663,7 +14663,7 @@
         <v>46</v>
       </c>
       <c r="I65">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -15095,10 +15095,10 @@
         <v>1</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -15124,10 +15124,10 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I81">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -15269,10 +15269,10 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I86">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -29218,7 +29218,7 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I567">
         <v>7</v>
@@ -29508,10 +29508,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="I577">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29537,10 +29537,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I578">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29569,7 +29569,7 @@
         <v>115</v>
       </c>
       <c r="I579">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -29653,10 +29653,10 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="I582">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -29885,10 +29885,10 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I590">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -29914,7 +29914,7 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I591">
         <v>11</v>
@@ -31306,7 +31306,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I639">
         <v>27</v>
@@ -31335,10 +31335,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I640">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31364,10 +31364,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="I641">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32115,13 +32115,13 @@
         <v>3</v>
       </c>
       <c r="G667">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H667">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I667">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.35">
@@ -32524,10 +32524,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="I681">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -34090,10 +34090,10 @@
         <v>1</v>
       </c>
       <c r="H735">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I735">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.35">
@@ -34119,10 +34119,10 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I736">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.35">
@@ -34148,10 +34148,10 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I737">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="738" spans="1:9" x14ac:dyDescent="0.35">
@@ -34206,10 +34206,10 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I739">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.35">
@@ -34641,10 +34641,10 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I754">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="755" spans="1:9" x14ac:dyDescent="0.35">
@@ -34876,7 +34876,7 @@
         <v>15</v>
       </c>
       <c r="I762">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="763" spans="1:9" x14ac:dyDescent="0.35">
@@ -35308,10 +35308,10 @@
         <v>1</v>
       </c>
       <c r="H777">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I777">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.35">
@@ -35946,10 +35946,10 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I799">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.35">
@@ -36062,10 +36062,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I803">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -36091,7 +36091,7 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I804">
         <v>12</v>
@@ -37570,10 +37570,10 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I855">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.35">
@@ -39194,10 +39194,10 @@
         <v>1</v>
       </c>
       <c r="H911">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="I911">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.35">
@@ -39658,10 +39658,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="I927">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -39774,7 +39774,7 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I931">
         <v>1</v>
@@ -41456,10 +41456,10 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I989">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.35">
@@ -41659,10 +41659,10 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="I996">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.35">
@@ -41717,7 +41717,7 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I998">
         <v>13</v>
@@ -44617,7 +44617,7 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="I1098">
         <v>24</v>
@@ -44733,7 +44733,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I1102">
         <v>29</v>
@@ -45023,10 +45023,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I1112">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">
@@ -45400,10 +45400,10 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I1125">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1126" spans="1:9" x14ac:dyDescent="0.35">
@@ -45455,13 +45455,13 @@
         <v>3</v>
       </c>
       <c r="G1127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1127">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I1127">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1128" spans="1:9" x14ac:dyDescent="0.35">
@@ -45980,7 +45980,7 @@
         <v>1</v>
       </c>
       <c r="H1145">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I1145">
         <v>1</v>

</xml_diff>

<commit_message>
Add files via upload (#24)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45869B6E-444E-4127-B407-691C47D178B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17C379-FE73-43F8-8B1A-1851EE2F0835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12772,7 +12772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -14689,7 +14689,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I66">
         <v>13</v>
@@ -29508,7 +29508,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="I577">
         <v>27</v>
@@ -29540,7 +29540,7 @@
         <v>138</v>
       </c>
       <c r="I578">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -31335,10 +31335,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="I640">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31364,7 +31364,7 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I641">
         <v>52</v>
@@ -32118,10 +32118,10 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I667">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.35">
@@ -32524,7 +32524,7 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I681">
         <v>24</v>
@@ -38295,10 +38295,10 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I880">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -39165,10 +39165,10 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I910">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.35">
@@ -39658,10 +39658,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="I927">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -44733,10 +44733,10 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="I1102">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.35">
@@ -47894,7 +47894,7 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I1211">
         <v>32</v>

</xml_diff>

<commit_message>
Add files via upload (#25)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17C379-FE73-43F8-8B1A-1851EE2F0835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D516FFA3-8690-4269-AED1-53855967E684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12776,7 +12776,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14338,13 +14338,13 @@
         <v>3</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -14718,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -28899,7 +28899,7 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I556">
         <v>9</v>
@@ -31367,7 +31367,7 @@
         <v>161</v>
       </c>
       <c r="I641">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -35949,7 +35949,7 @@
         <v>64</v>
       </c>
       <c r="I799">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.35">
@@ -37744,7 +37744,7 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I861">
         <v>9</v>
@@ -44733,10 +44733,10 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I1102">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#26)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D516FFA3-8690-4269-AED1-53855967E684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC381110-5EA6-4A5F-BB73-33980AF8F1DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12772,11 +12772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
+      <selection activeCell="J681" sqref="J681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32524,10 +32524,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I681">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#27)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC381110-5EA6-4A5F-BB73-33980AF8F1DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA8E0FC8-D612-4084-BCBC-E3D54C33F1A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6910"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -11938,7 +11938,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12772,11 +12772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
-      <selection activeCell="J681" sqref="J681"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15269,7 +15269,7 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I86">
         <v>13</v>
@@ -22606,10 +22606,10 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="I339">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.35">
@@ -29508,10 +29508,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="I577">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29537,10 +29537,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I578">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -31338,7 +31338,7 @@
         <v>54</v>
       </c>
       <c r="I640">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31364,10 +31364,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="I641">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32524,10 +32524,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="I681">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -37744,10 +37744,10 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I861">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -39397,10 +39397,10 @@
         <v>1</v>
       </c>
       <c r="H918">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I918">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.35">
@@ -39774,7 +39774,7 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I931">
         <v>1</v>

</xml_diff>

<commit_message>
Add files via upload (#28)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA8E0FC8-D612-4084-BCBC-E3D54C33F1A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F1E49FB-75A0-445C-B2F1-4F2FDB5D2B73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -14660,7 +14660,7 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I65">
         <v>15</v>
@@ -14802,13 +14802,13 @@
         <v>3</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -15124,10 +15124,10 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="I81">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -15153,10 +15153,10 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="I82">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -22606,7 +22606,7 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I339">
         <v>17</v>
@@ -29218,7 +29218,7 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I567">
         <v>7</v>
@@ -29508,10 +29508,10 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="I577">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -29537,10 +29537,10 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="I578">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -29885,7 +29885,7 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="I590">
         <v>10</v>
@@ -31306,7 +31306,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I639">
         <v>27</v>
@@ -31364,7 +31364,7 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="I641">
         <v>55</v>
@@ -32118,7 +32118,7 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I667">
         <v>4</v>
@@ -32408,7 +32408,7 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="I677">
         <v>6</v>
@@ -32524,10 +32524,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I681">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -34583,10 +34583,10 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I752">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.35">
@@ -34641,7 +34641,7 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I754">
         <v>5</v>
@@ -34873,7 +34873,7 @@
         <v>1</v>
       </c>
       <c r="H762">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I762">
         <v>5</v>
@@ -35946,7 +35946,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I799">
         <v>22</v>
@@ -38295,7 +38295,7 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I880">
         <v>19</v>
@@ -39658,10 +39658,10 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I927">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.35">
@@ -39774,7 +39774,7 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I931">
         <v>1</v>
@@ -41717,7 +41717,7 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I998">
         <v>13</v>
@@ -44385,7 +44385,7 @@
         <v>1</v>
       </c>
       <c r="H1090">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I1090">
         <v>1</v>
@@ -44617,7 +44617,7 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I1098">
         <v>24</v>
@@ -44733,7 +44733,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I1102">
         <v>32</v>
@@ -44962,13 +44962,13 @@
         <v>3</v>
       </c>
       <c r="G1110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1110">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I1110">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1111" spans="1:9" x14ac:dyDescent="0.35">
@@ -45023,10 +45023,10 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="I1112">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.35">
@@ -45400,7 +45400,7 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I1125">
         <v>2</v>
@@ -45429,10 +45429,10 @@
         <v>1</v>
       </c>
       <c r="H1126">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I1126">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1127" spans="1:9" x14ac:dyDescent="0.35">
@@ -46009,7 +46009,7 @@
         <v>1</v>
       </c>
       <c r="H1146">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I1146">
         <v>1</v>
@@ -47894,10 +47894,10 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I1211">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1212" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#29)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F1E49FB-75A0-445C-B2F1-4F2FDB5D2B73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7733C1-C53F-4319-96B9-5591CBB2AE50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -13326,7 +13326,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -14341,7 +14341,7 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -14660,7 +14660,7 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="I65">
         <v>15</v>
@@ -14718,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -15095,7 +15095,7 @@
         <v>1</v>
       </c>
       <c r="H80">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -15124,7 +15124,7 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I81">
         <v>8</v>
@@ -15153,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="I82">
         <v>6</v>
@@ -15269,7 +15269,7 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="I86">
         <v>13</v>
@@ -22606,7 +22606,7 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="I339">
         <v>17</v>
@@ -25915,7 +25915,7 @@
         <v>11</v>
       </c>
       <c r="I453">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.35">
@@ -27884,7 +27884,7 @@
         <v>1</v>
       </c>
       <c r="H521">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I521">
         <v>3</v>
@@ -28899,7 +28899,7 @@
         <v>1</v>
       </c>
       <c r="H556">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I556">
         <v>9</v>
@@ -29218,7 +29218,7 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I567">
         <v>7</v>
@@ -29508,7 +29508,7 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="I577">
         <v>30</v>
@@ -29537,7 +29537,7 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="I578">
         <v>30</v>
@@ -29566,7 +29566,7 @@
         <v>1</v>
       </c>
       <c r="H579">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="I579">
         <v>13</v>
@@ -29653,7 +29653,7 @@
         <v>1</v>
       </c>
       <c r="H582">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="I582">
         <v>16</v>
@@ -29885,7 +29885,7 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="I590">
         <v>10</v>
@@ -29914,7 +29914,7 @@
         <v>1</v>
       </c>
       <c r="H591">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I591">
         <v>11</v>
@@ -29972,7 +29972,7 @@
         <v>1</v>
       </c>
       <c r="H593">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I593">
         <v>1</v>
@@ -30059,7 +30059,7 @@
         <v>1</v>
       </c>
       <c r="H596">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I596">
         <v>2</v>
@@ -31306,7 +31306,7 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="I639">
         <v>27</v>
@@ -31335,10 +31335,10 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I640">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -31364,10 +31364,10 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>190</v>
+        <v>246</v>
       </c>
       <c r="I641">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32118,10 +32118,10 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I667">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.35">
@@ -32408,7 +32408,7 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I677">
         <v>6</v>
@@ -32524,7 +32524,7 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="I681">
         <v>28</v>
@@ -33133,7 +33133,7 @@
         <v>1</v>
       </c>
       <c r="H702">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I702">
         <v>1</v>
@@ -33191,7 +33191,7 @@
         <v>1</v>
       </c>
       <c r="H704">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I704">
         <v>2</v>
@@ -33336,7 +33336,7 @@
         <v>1</v>
       </c>
       <c r="H709">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I709">
         <v>1</v>
@@ -33974,7 +33974,7 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I731">
         <v>4</v>
@@ -34003,7 +34003,7 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I732">
         <v>4</v>
@@ -34032,7 +34032,7 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I733">
         <v>4</v>
@@ -34061,7 +34061,7 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I734">
         <v>4</v>
@@ -34090,7 +34090,7 @@
         <v>1</v>
       </c>
       <c r="H735">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I735">
         <v>6</v>
@@ -34119,7 +34119,7 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I736">
         <v>6</v>
@@ -34148,7 +34148,7 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I737">
         <v>6</v>
@@ -34206,7 +34206,7 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I739">
         <v>7</v>
@@ -34554,7 +34554,7 @@
         <v>1</v>
       </c>
       <c r="H751">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I751">
         <v>4</v>
@@ -34583,7 +34583,7 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I752">
         <v>6</v>
@@ -34612,7 +34612,7 @@
         <v>1</v>
       </c>
       <c r="H753">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I753">
         <v>5</v>
@@ -34641,7 +34641,7 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I754">
         <v>5</v>
@@ -34873,7 +34873,7 @@
         <v>1</v>
       </c>
       <c r="H762">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I762">
         <v>5</v>
@@ -35946,7 +35946,7 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="I799">
         <v>22</v>
@@ -35975,7 +35975,7 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I800">
         <v>4</v>
@@ -36062,10 +36062,10 @@
         <v>1</v>
       </c>
       <c r="H803">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="I803">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -36091,7 +36091,7 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I804">
         <v>12</v>
@@ -37048,7 +37048,7 @@
         <v>1</v>
       </c>
       <c r="H837">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I837">
         <v>1</v>
@@ -37570,7 +37570,7 @@
         <v>1</v>
       </c>
       <c r="H855">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I855">
         <v>5</v>
@@ -37744,10 +37744,10 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="I861">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -38295,7 +38295,7 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="I880">
         <v>19</v>
@@ -39020,7 +39020,7 @@
         <v>1</v>
       </c>
       <c r="H905">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I905">
         <v>1</v>
@@ -39136,7 +39136,7 @@
         <v>1</v>
       </c>
       <c r="H909">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I909">
         <v>2</v>
@@ -39165,7 +39165,7 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="I910">
         <v>19</v>
@@ -39194,7 +39194,7 @@
         <v>1</v>
       </c>
       <c r="H911">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="I911">
         <v>24</v>
@@ -39397,7 +39397,7 @@
         <v>1</v>
       </c>
       <c r="H918">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I918">
         <v>7</v>
@@ -39629,7 +39629,7 @@
         <v>1</v>
       </c>
       <c r="H926">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I926">
         <v>1</v>
@@ -39658,7 +39658,7 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="I927">
         <v>29</v>
@@ -40122,7 +40122,7 @@
         <v>1</v>
       </c>
       <c r="H943">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="I943">
         <v>7</v>
@@ -40760,7 +40760,7 @@
         <v>1</v>
       </c>
       <c r="H965">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I965">
         <v>1</v>
@@ -41079,7 +41079,7 @@
         <v>1</v>
       </c>
       <c r="H976">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I976">
         <v>1</v>
@@ -41108,7 +41108,7 @@
         <v>1</v>
       </c>
       <c r="H977">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I977">
         <v>2</v>
@@ -41166,7 +41166,7 @@
         <v>1</v>
       </c>
       <c r="H979">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I979">
         <v>5</v>
@@ -41195,7 +41195,7 @@
         <v>1</v>
       </c>
       <c r="H980">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="I980">
         <v>5</v>
@@ -41456,7 +41456,7 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="I989">
         <v>14</v>
@@ -41659,7 +41659,7 @@
         <v>1</v>
       </c>
       <c r="H996">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="I996">
         <v>24</v>
@@ -41717,7 +41717,7 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="I998">
         <v>13</v>
@@ -44617,7 +44617,7 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="I1098">
         <v>24</v>
@@ -44733,7 +44733,7 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="I1102">
         <v>32</v>
@@ -45023,7 +45023,7 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="I1112">
         <v>19</v>
@@ -45371,7 +45371,7 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I1124">
         <v>6</v>
@@ -45400,7 +45400,7 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1125">
         <v>2</v>
@@ -45429,7 +45429,7 @@
         <v>1</v>
       </c>
       <c r="H1126">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I1126">
         <v>3</v>
@@ -45458,7 +45458,7 @@
         <v>1</v>
       </c>
       <c r="H1127">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1127">
         <v>2</v>
@@ -45487,7 +45487,7 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I1128">
         <v>3</v>
@@ -45690,7 +45690,7 @@
         <v>1</v>
       </c>
       <c r="H1135">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="I1135">
         <v>9</v>
@@ -46009,7 +46009,7 @@
         <v>1</v>
       </c>
       <c r="H1146">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1146">
         <v>1</v>
@@ -46502,7 +46502,7 @@
         <v>1</v>
       </c>
       <c r="H1163">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1163">
         <v>1</v>
@@ -47894,7 +47894,7 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="I1211">
         <v>33</v>

</xml_diff>

<commit_message>
Add files via upload (#30)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7733C1-C53F-4319-96B9-5591CBB2AE50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{91A41360-4A9E-4054-9FB6-A9B9E75A34AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12776,7 +12776,7 @@
   <dimension ref="A1:I1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31367,7 +31367,7 @@
         <v>246</v>
       </c>
       <c r="I641">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -32524,10 +32524,10 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="I681">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -36065,7 +36065,7 @@
         <v>55</v>
       </c>
       <c r="I803">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -37747,7 +37747,7 @@
         <v>98</v>
       </c>
       <c r="I861">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -39658,7 +39658,7 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I927">
         <v>29</v>
@@ -41253,10 +41253,10 @@
         <v>1</v>
       </c>
       <c r="H982">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I982">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="983" spans="1:9" x14ac:dyDescent="0.35">
@@ -41456,7 +41456,7 @@
         <v>1</v>
       </c>
       <c r="H989">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I989">
         <v>14</v>
@@ -44733,10 +44733,10 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="I1102">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#32)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8177E5E0-F85F-45C7-A0DF-D36FF3A87FBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB1DC026-89E7-4BC9-83CD-0D7F4C8553F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12779,7 +12779,7 @@
   <dimension ref="A1:J1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14887,13 +14887,13 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I66">
         <v>13</v>
       </c>
       <c r="J66">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -15533,7 +15533,7 @@
         <v>13</v>
       </c>
       <c r="J86">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -33223,13 +33223,13 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I639">
         <v>27</v>
       </c>
       <c r="J639">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.35">
@@ -33287,13 +33287,13 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="I641">
         <v>56</v>
       </c>
       <c r="J641">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.35">
@@ -36423,13 +36423,13 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I739">
         <v>7</v>
       </c>
       <c r="J739">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="740" spans="1:10" x14ac:dyDescent="0.35">
@@ -41895,13 +41895,13 @@
         <v>1</v>
       </c>
       <c r="H910">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I910">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J910">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="911" spans="1:10" x14ac:dyDescent="0.35">
@@ -48871,13 +48871,13 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I1128">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1128">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1129" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#33)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB1DC026-89E7-4BC9-83CD-0D7F4C8553F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{952CC38A-F2CF-49BE-A605-44296CD0C1E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12779,7 +12779,7 @@
   <dimension ref="A1:J1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15335,13 +15335,13 @@
         <v>1</v>
       </c>
       <c r="H80">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -33287,13 +33287,13 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I641">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J641">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.35">
@@ -34119,13 +34119,13 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="I667">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J667">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.35">
@@ -36423,13 +36423,13 @@
         <v>1</v>
       </c>
       <c r="H739">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I739">
         <v>7</v>
       </c>
       <c r="J739">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="740" spans="1:10" x14ac:dyDescent="0.35">
@@ -42439,13 +42439,13 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I927">
         <v>29</v>
       </c>
       <c r="J927">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="928" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#34)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{952CC38A-F2CF-49BE-A605-44296CD0C1E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45C3B512-06E0-42E2-AC57-E1884365DD77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -15399,13 +15399,13 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="I82">
         <v>6</v>
       </c>
       <c r="J82">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -34442,7 +34442,7 @@
         <v>61</v>
       </c>
       <c r="I677">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J677">
         <v>7</v>
@@ -48039,13 +48039,13 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I1102">
         <v>33</v>
       </c>
       <c r="J1102">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#35)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45C3B512-06E0-42E2-AC57-E1884365DD77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87A7807D-5AB2-47E5-99EA-709FA47F1E05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12779,7 +12779,7 @@
   <dimension ref="A1:J1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38375,13 +38375,13 @@
         <v>1</v>
       </c>
       <c r="H800">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I800">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J800">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="801" spans="1:10" x14ac:dyDescent="0.35">
@@ -42407,13 +42407,13 @@
         <v>1</v>
       </c>
       <c r="H926">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I926">
         <v>1</v>
       </c>
       <c r="J926">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="927" spans="1:10" x14ac:dyDescent="0.35">
@@ -48039,13 +48039,13 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I1102">
         <v>33</v>
       </c>
       <c r="J1102">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">
@@ -48871,7 +48871,7 @@
         <v>1</v>
       </c>
       <c r="H1128">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I1128">
         <v>4</v>
@@ -49095,13 +49095,13 @@
         <v>1</v>
       </c>
       <c r="H1135">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I1135">
         <v>9</v>
       </c>
       <c r="J1135">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1136" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#36)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87A7807D-5AB2-47E5-99EA-709FA47F1E05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E64325B-ACFF-41D8-A113-33083C698C1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
@@ -12778,8 +12778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A721" workbookViewId="0">
+      <selection activeCell="A731" sqref="A731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36167,13 +36167,13 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I731">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J731">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="732" spans="1:10" x14ac:dyDescent="0.35">
@@ -36199,13 +36199,13 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="I732">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J732">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.35">
@@ -36231,13 +36231,13 @@
         <v>1</v>
       </c>
       <c r="H733">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="I733">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J733">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="734" spans="1:10" x14ac:dyDescent="0.35">
@@ -36263,13 +36263,13 @@
         <v>0</v>
       </c>
       <c r="H734">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="I734">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J734">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:10" x14ac:dyDescent="0.35">
@@ -36295,13 +36295,13 @@
         <v>1</v>
       </c>
       <c r="H735">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I735">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J735">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="736" spans="1:10" x14ac:dyDescent="0.35">
@@ -36327,13 +36327,13 @@
         <v>1</v>
       </c>
       <c r="H736">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="I736">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J736">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="737" spans="1:10" x14ac:dyDescent="0.35">
@@ -36359,13 +36359,13 @@
         <v>1</v>
       </c>
       <c r="H737">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="I737">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J737">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="738" spans="1:10" x14ac:dyDescent="0.35">
@@ -42573,7 +42573,7 @@
         <v>1</v>
       </c>
       <c r="J931">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="932" spans="1:10" x14ac:dyDescent="0.35">
@@ -48807,13 +48807,13 @@
         <v>1</v>
       </c>
       <c r="H1126">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1126">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1126">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1127" spans="1:10" x14ac:dyDescent="0.35">
@@ -48839,13 +48839,13 @@
         <v>1</v>
       </c>
       <c r="H1127">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I1127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J1127">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1128" spans="1:10" x14ac:dyDescent="0.35">
@@ -51527,13 +51527,13 @@
         <v>1</v>
       </c>
       <c r="H1211">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I1211">
         <v>33</v>
       </c>
       <c r="J1211">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="1212" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#37)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agwilso2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E64325B-ACFF-41D8-A113-33083C698C1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -12004,7 +12003,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -12397,27 +12396,27 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -12496,7 +12495,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -12508,7 +12507,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -12555,23 +12554,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -12607,23 +12589,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -12778,8 +12743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A721" workbookViewId="0">
-      <selection activeCell="A731" sqref="A731"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15402,7 +15367,7 @@
         <v>157</v>
       </c>
       <c r="I82">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J82">
         <v>102</v>
@@ -15527,13 +15492,13 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I86">
         <v>13</v>
       </c>
       <c r="J86">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -30570,10 +30535,10 @@
         <v>26</v>
       </c>
       <c r="I556">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J556">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="557" spans="1:10" x14ac:dyDescent="0.35">
@@ -33290,7 +33255,7 @@
         <v>264</v>
       </c>
       <c r="I641">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J641">
         <v>153</v>
@@ -34119,13 +34084,13 @@
         <v>1</v>
       </c>
       <c r="H667">
+        <v>164</v>
+      </c>
+      <c r="I667">
+        <v>17</v>
+      </c>
+      <c r="J667">
         <v>99</v>
-      </c>
-      <c r="I667">
-        <v>11</v>
-      </c>
-      <c r="J667">
-        <v>49</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.35">
@@ -41898,7 +41863,7 @@
         <v>139</v>
       </c>
       <c r="I910">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J910">
         <v>68</v>
@@ -42413,7 +42378,7 @@
         <v>1</v>
       </c>
       <c r="J926">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="927" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#39)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -12743,8 +12743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A38" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13956,13 +13956,13 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -33220,13 +33220,13 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I640">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J640">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.35">
@@ -33252,13 +33252,13 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="I641">
         <v>58</v>
       </c>
       <c r="J641">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.35">
@@ -34084,13 +34084,13 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="I667">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J667">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.35">
@@ -42538,7 +42538,7 @@
         <v>1</v>
       </c>
       <c r="J931">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="932" spans="1:10" x14ac:dyDescent="0.35">
@@ -44676,13 +44676,13 @@
         <v>1</v>
       </c>
       <c r="H998">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="I998">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J998">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="999" spans="1:10" x14ac:dyDescent="0.35">
@@ -48004,13 +48004,13 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I1102">
         <v>33</v>
       </c>
       <c r="J1102">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#41)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -12743,8 +12743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A38" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33220,13 +33220,13 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I640">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J640">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.35">
@@ -34084,13 +34084,13 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="I667">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J667">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.35">
@@ -36164,13 +36164,13 @@
         <v>1</v>
       </c>
       <c r="H732">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="I732">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J732">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.35">
@@ -38468,13 +38468,13 @@
         <v>1</v>
       </c>
       <c r="H804">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I804">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J804">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="805" spans="1:10" x14ac:dyDescent="0.35">
@@ -47876,13 +47876,13 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="I1098">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J1098">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="1099" spans="1:10" x14ac:dyDescent="0.35">
@@ -48004,13 +48004,13 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I1102">
         <v>33</v>
       </c>
       <c r="J1102">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">
@@ -48740,13 +48740,13 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I1125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1125">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1126" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add files via upload (#42)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -39527,7 +39527,7 @@
         <v>8</v>
       </c>
       <c r="I837">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J837">
         <v>5</v>

</xml_diff>

<commit_message>
Add files via upload (#43)
</commit_message>
<xml_diff>
--- a/data/CGA.xlsx
+++ b/data/CGA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
   </bookViews>
   <sheets>
     <sheet name="CtByBldg" sheetId="1" r:id="rId1"/>
@@ -12744,7 +12744,7 @@
   <dimension ref="A1:J1225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14820,13 +14820,13 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="I65">
         <v>15</v>
       </c>
       <c r="J65">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -14858,7 +14858,7 @@
         <v>13</v>
       </c>
       <c r="J66">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -14890,7 +14890,7 @@
         <v>10</v>
       </c>
       <c r="J67">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -15364,13 +15364,13 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="I82">
         <v>7</v>
       </c>
       <c r="J82">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -15492,13 +15492,13 @@
         <v>1</v>
       </c>
       <c r="H86">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I86">
         <v>13</v>
       </c>
       <c r="J86">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -23588,7 +23588,7 @@
         <v>1</v>
       </c>
       <c r="H339">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="I339">
         <v>17</v>
@@ -27236,7 +27236,7 @@
         <v>1</v>
       </c>
       <c r="H453">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I453">
         <v>3</v>
@@ -30884,13 +30884,13 @@
         <v>1</v>
       </c>
       <c r="H567">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I567">
         <v>7</v>
       </c>
       <c r="J567">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.35">
@@ -31204,13 +31204,13 @@
         <v>1</v>
       </c>
       <c r="H577">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="I577">
         <v>30</v>
       </c>
       <c r="J577">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="578" spans="1:10" x14ac:dyDescent="0.35">
@@ -31236,13 +31236,13 @@
         <v>1</v>
       </c>
       <c r="H578">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="I578">
         <v>30</v>
       </c>
       <c r="J578">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="579" spans="1:10" x14ac:dyDescent="0.35">
@@ -31274,7 +31274,7 @@
         <v>13</v>
       </c>
       <c r="J579">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="580" spans="1:10" x14ac:dyDescent="0.35">
@@ -31370,7 +31370,7 @@
         <v>16</v>
       </c>
       <c r="J582">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="583" spans="1:10" x14ac:dyDescent="0.35">
@@ -31620,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H590">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="I590">
         <v>10</v>
@@ -31658,7 +31658,7 @@
         <v>11</v>
       </c>
       <c r="J591">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.35">
@@ -33188,13 +33188,13 @@
         <v>1</v>
       </c>
       <c r="H639">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="I639">
         <v>27</v>
       </c>
       <c r="J639">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.35">
@@ -33220,13 +33220,13 @@
         <v>1</v>
       </c>
       <c r="H640">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="I640">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J640">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.35">
@@ -33252,13 +33252,13 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="I641">
         <v>58</v>
       </c>
       <c r="J641">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.35">
@@ -34084,13 +34084,13 @@
         <v>1</v>
       </c>
       <c r="H667">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="I667">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J667">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.35">
@@ -34404,7 +34404,7 @@
         <v>1</v>
       </c>
       <c r="H677">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I677">
         <v>7</v>
@@ -34532,13 +34532,13 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I681">
         <v>29</v>
       </c>
       <c r="J681">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="682" spans="1:10" x14ac:dyDescent="0.35">
@@ -35268,13 +35268,13 @@
         <v>1</v>
       </c>
       <c r="H704">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I704">
+        <v>1</v>
+      </c>
+      <c r="J704">
         <v>2</v>
-      </c>
-      <c r="J704">
-        <v>3</v>
       </c>
     </row>
     <row r="705" spans="1:10" x14ac:dyDescent="0.35">
@@ -36132,7 +36132,7 @@
         <v>1</v>
       </c>
       <c r="H731">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I731">
         <v>2</v>
@@ -36772,7 +36772,7 @@
         <v>1</v>
       </c>
       <c r="H751">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I751">
         <v>4</v>
@@ -36804,13 +36804,13 @@
         <v>1</v>
       </c>
       <c r="H752">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I752">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J752">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="753" spans="1:10" x14ac:dyDescent="0.35">
@@ -36868,13 +36868,13 @@
         <v>1</v>
       </c>
       <c r="H754">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I754">
         <v>5</v>
       </c>
       <c r="J754">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="755" spans="1:10" x14ac:dyDescent="0.35">
@@ -37124,7 +37124,7 @@
         <v>1</v>
       </c>
       <c r="H762">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="I762">
         <v>5</v>
@@ -38308,13 +38308,13 @@
         <v>1</v>
       </c>
       <c r="H799">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I799">
         <v>22</v>
       </c>
       <c r="J799">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="800" spans="1:10" x14ac:dyDescent="0.35">
@@ -40106,7 +40106,7 @@
         <v>5</v>
       </c>
       <c r="J855">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="856" spans="1:10" x14ac:dyDescent="0.35">
@@ -40292,7 +40292,7 @@
         <v>1</v>
       </c>
       <c r="H861">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="I861">
         <v>10</v>
@@ -40900,13 +40900,13 @@
         <v>1</v>
       </c>
       <c r="H880">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="I880">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J880">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="881" spans="1:10" x14ac:dyDescent="0.35">
@@ -41866,7 +41866,7 @@
         <v>21</v>
       </c>
       <c r="J910">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="911" spans="1:10" x14ac:dyDescent="0.35">
@@ -42404,7 +42404,7 @@
         <v>1</v>
       </c>
       <c r="H927">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I927">
         <v>29</v>
@@ -42532,7 +42532,7 @@
         <v>1</v>
       </c>
       <c r="H931">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I931">
         <v>1</v>
@@ -44100,13 +44100,13 @@
         <v>1</v>
       </c>
       <c r="H980">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I980">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J980">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="981" spans="1:10" x14ac:dyDescent="0.35">
@@ -44164,7 +44164,7 @@
         <v>1</v>
       </c>
       <c r="H982">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I982">
         <v>1</v>
@@ -44394,7 +44394,7 @@
         <v>14</v>
       </c>
       <c r="J989">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="990" spans="1:10" x14ac:dyDescent="0.35">
@@ -44618,7 +44618,7 @@
         <v>24</v>
       </c>
       <c r="J996">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="997" spans="1:10" x14ac:dyDescent="0.35">
@@ -47620,7 +47620,7 @@
         <v>1</v>
       </c>
       <c r="H1090">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I1090">
         <v>1</v>
@@ -47876,13 +47876,13 @@
         <v>1</v>
       </c>
       <c r="H1098">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="I1098">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1098">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="1099" spans="1:10" x14ac:dyDescent="0.35">
@@ -48004,13 +48004,13 @@
         <v>1</v>
       </c>
       <c r="H1102">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="I1102">
         <v>33</v>
       </c>
       <c r="J1102">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.35">
@@ -48260,7 +48260,7 @@
         <v>1</v>
       </c>
       <c r="H1110">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1110">
         <v>2</v>
@@ -48324,13 +48324,13 @@
         <v>1</v>
       </c>
       <c r="H1112">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="I1112">
         <v>19</v>
       </c>
       <c r="J1112">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="1113" spans="1:10" x14ac:dyDescent="0.35">
@@ -48708,13 +48708,13 @@
         <v>1</v>
       </c>
       <c r="H1124">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I1124">
         <v>6</v>
       </c>
       <c r="J1124">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1125" spans="1:10" x14ac:dyDescent="0.35">
@@ -48740,7 +48740,7 @@
         <v>1</v>
       </c>
       <c r="H1125">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I1125">
         <v>3</v>
@@ -49418,7 +49418,7 @@
         <v>1</v>
       </c>
       <c r="J1146">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1147" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>